<commit_message>
Updates to est/mort tables and barplot code
-est/mort tables have been doublechecked
-all species are in the same order as initial grid
-colors in barplot code are updated to Jenneke's color ramp
</commit_message>
<xml_diff>
--- a/LaVegMod3_Mortality_Tables_v01_01.xlsx
+++ b/LaVegMod3_Mortality_Tables_v01_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\Coastal Hydro Dropbox\Madeline Foster-Martinez\MRF_LAVegMod\updates_for_G030\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\Documents\GitHub\ICM_LAVegMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556852DF-5BB0-437A-9B7B-87DF70D9D932}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9AB0A-0A6D-4AE8-B7B1-096D37C95457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="28" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="1380" windowWidth="21600" windowHeight="11205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="28" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="172">
   <si>
     <t>WAXM</t>
   </si>
@@ -420,12 +420,6 @@
   </si>
   <si>
     <t>OpenWater</t>
-  </si>
-  <si>
-    <t>SAV</t>
-  </si>
-  <si>
-    <t>SAVModel</t>
   </si>
   <si>
     <t>BarrierIslandModel</t>
@@ -2240,9 +2234,9 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="11.44140625" style="37"/>
+    <col min="1" max="4" width="11.42578125" style="37"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2266,28 +2260,28 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="2" customWidth="1"/>
     <col min="15" max="15" width="6" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" style="2" customWidth="1"/>
-    <col min="17" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.6640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.44140625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="2"/>
+    <col min="16" max="16" width="6.28515625" style="2" customWidth="1"/>
+    <col min="17" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -2320,7 +2314,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="39" t="s">
         <v>6</v>
@@ -4415,28 +4409,28 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="2" customWidth="1"/>
     <col min="15" max="15" width="6" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" style="2" customWidth="1"/>
-    <col min="17" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.6640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.44140625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="2"/>
+    <col min="16" max="16" width="6.28515625" style="2" customWidth="1"/>
+    <col min="17" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -4469,7 +4463,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="39" t="s">
         <v>6</v>
@@ -6565,14 +6559,14 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="19" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="19" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -6605,10 +6599,10 @@
       <c r="W1" s="203"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="14.4" thickBot="1">
+    <row r="2" spans="1:24" ht="15" thickBot="1">
       <c r="A2" s="202"/>
       <c r="B2" s="166" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="167">
         <v>0</v>
@@ -6674,7 +6668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="13.8">
+    <row r="3" spans="1:24" ht="14.25">
       <c r="A3" s="202"/>
       <c r="B3" s="172">
         <v>0</v>
@@ -6743,7 +6737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="13.8">
+    <row r="4" spans="1:24" ht="14.25">
       <c r="A4" s="202"/>
       <c r="B4" s="177">
         <v>0.2</v>
@@ -6812,7 +6806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="13.8">
+    <row r="5" spans="1:24" ht="14.25">
       <c r="A5" s="202"/>
       <c r="B5" s="180">
         <v>0.4</v>
@@ -6881,7 +6875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="13.8">
+    <row r="6" spans="1:24" ht="14.25">
       <c r="A6" s="202"/>
       <c r="B6" s="181">
         <v>0.6</v>
@@ -6950,7 +6944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="3" customFormat="1" ht="13.8">
+    <row r="7" spans="1:24" s="3" customFormat="1" ht="14.25">
       <c r="A7" s="202"/>
       <c r="B7" s="181">
         <v>0.8</v>
@@ -7019,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="13.8">
+    <row r="8" spans="1:24" ht="14.25">
       <c r="A8" s="202"/>
       <c r="B8" s="182">
         <v>1</v>
@@ -7088,7 +7082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="13.8">
+    <row r="9" spans="1:24" ht="14.25">
       <c r="A9" s="202"/>
       <c r="B9" s="182">
         <v>1.2</v>
@@ -7157,7 +7151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="13.8">
+    <row r="10" spans="1:24" ht="14.25">
       <c r="A10" s="202"/>
       <c r="B10" s="182">
         <v>1.4</v>
@@ -7226,7 +7220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="13.8">
+    <row r="11" spans="1:24" ht="14.25">
       <c r="A11" s="202"/>
       <c r="B11" s="182">
         <v>1.6</v>
@@ -7295,7 +7289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="13.8">
+    <row r="12" spans="1:24" ht="14.25">
       <c r="A12" s="202"/>
       <c r="B12" s="182">
         <v>1.8</v>
@@ -7364,7 +7358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="13.8">
+    <row r="13" spans="1:24" ht="14.25">
       <c r="A13" s="202"/>
       <c r="B13" s="182">
         <v>2</v>
@@ -7433,7 +7427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="13.8">
+    <row r="14" spans="1:24" ht="14.25">
       <c r="A14" s="202"/>
       <c r="B14" s="182">
         <v>3</v>
@@ -7502,7 +7496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="13.8">
+    <row r="15" spans="1:24" ht="14.25">
       <c r="A15" s="202"/>
       <c r="B15" s="182">
         <v>4</v>
@@ -7571,7 +7565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="13.8">
+    <row r="16" spans="1:24" ht="14.25">
       <c r="A16" s="202"/>
       <c r="B16" s="182">
         <v>5</v>
@@ -7640,7 +7634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="13.8">
+    <row r="17" spans="1:23" ht="14.25">
       <c r="A17" s="202"/>
       <c r="B17" s="184">
         <v>6</v>
@@ -7709,7 +7703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="13.8">
+    <row r="18" spans="1:23" ht="14.25">
       <c r="A18" s="202"/>
       <c r="B18" s="184">
         <v>7</v>
@@ -7778,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="13.8">
+    <row r="19" spans="1:23" ht="14.25">
       <c r="A19" s="202"/>
       <c r="B19" s="184">
         <v>8</v>
@@ -7847,7 +7841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="13.8">
+    <row r="20" spans="1:23" ht="14.25">
       <c r="A20" s="202"/>
       <c r="B20" s="184">
         <v>9</v>
@@ -7916,7 +7910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="13.8">
+    <row r="21" spans="1:23" ht="14.25">
       <c r="A21" s="202"/>
       <c r="B21" s="184">
         <v>10</v>
@@ -7985,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="13.8">
+    <row r="22" spans="1:23" ht="14.25">
       <c r="A22" s="202"/>
       <c r="B22" s="184">
         <v>12</v>
@@ -8054,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="13.8">
+    <row r="23" spans="1:23" ht="14.25">
       <c r="A23" s="202"/>
       <c r="B23" s="184">
         <v>14</v>
@@ -8123,7 +8117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="13.8">
+    <row r="24" spans="1:23" ht="14.25">
       <c r="A24" s="202"/>
       <c r="B24" s="184">
         <v>16</v>
@@ -8192,7 +8186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="13.8">
+    <row r="25" spans="1:23" ht="14.25">
       <c r="A25" s="202"/>
       <c r="B25" s="184">
         <v>18</v>
@@ -8261,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="13.8">
+    <row r="26" spans="1:23" ht="14.25">
       <c r="A26" s="202"/>
       <c r="B26" s="184">
         <v>20</v>
@@ -8330,7 +8324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="13.8">
+    <row r="27" spans="1:23" ht="14.25">
       <c r="A27" s="202"/>
       <c r="B27" s="184">
         <v>22</v>
@@ -8399,7 +8393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="13.8">
+    <row r="28" spans="1:23" ht="14.25">
       <c r="A28" s="202"/>
       <c r="B28" s="184">
         <v>24</v>
@@ -8468,7 +8462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="13.8">
+    <row r="29" spans="1:23" ht="14.25">
       <c r="A29" s="202"/>
       <c r="B29" s="184">
         <v>26</v>
@@ -8537,7 +8531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="13.8">
+    <row r="30" spans="1:23" ht="14.25">
       <c r="A30" s="202"/>
       <c r="B30" s="184">
         <v>28</v>
@@ -8606,7 +8600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="13.8">
+    <row r="31" spans="1:23" ht="14.25">
       <c r="A31" s="202"/>
       <c r="B31" s="184">
         <v>100</v>
@@ -8696,16 +8690,16 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="8.109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="6.44140625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="6.42578125" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -8738,7 +8732,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="76" t="s">
         <v>0</v>
@@ -10833,28 +10827,28 @@
       <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="2" customWidth="1"/>
     <col min="13" max="13" width="7" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.44140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="2" customWidth="1"/>
     <col min="15" max="15" width="6" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" style="2" customWidth="1"/>
-    <col min="17" max="19" width="5.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.6640625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.44140625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="2"/>
+    <col min="16" max="16" width="6.28515625" style="2" customWidth="1"/>
+    <col min="17" max="19" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" style="2" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -10887,7 +10881,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="39" t="s">
         <v>6</v>
@@ -12983,16 +12977,16 @@
       <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="22" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -13025,7 +13019,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="75" t="s">
         <v>46</v>
@@ -13094,7 +13088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="12.9" customHeight="1">
+    <row r="3" spans="1:24" ht="12.95" customHeight="1">
       <c r="A3" s="198"/>
       <c r="B3" s="12">
         <v>0</v>
@@ -13163,7 +13157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="12.9" customHeight="1">
+    <row r="4" spans="1:24" ht="12.95" customHeight="1">
       <c r="A4" s="198"/>
       <c r="B4" s="24">
         <v>0.2</v>
@@ -13232,7 +13226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12.9" customHeight="1">
+    <row r="5" spans="1:24" ht="12.95" customHeight="1">
       <c r="A5" s="198"/>
       <c r="B5" s="26">
         <v>0.4</v>
@@ -13301,7 +13295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12.9" customHeight="1">
+    <row r="6" spans="1:24" ht="12.95" customHeight="1">
       <c r="A6" s="198"/>
       <c r="B6" s="26">
         <v>0.6</v>
@@ -13370,7 +13364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="12.9" customHeight="1">
+    <row r="7" spans="1:24" ht="12.95" customHeight="1">
       <c r="A7" s="198"/>
       <c r="B7" s="14">
         <v>0.8</v>
@@ -13439,7 +13433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="12.9" customHeight="1">
+    <row r="8" spans="1:24" ht="12.95" customHeight="1">
       <c r="A8" s="198"/>
       <c r="B8" s="14">
         <v>1</v>
@@ -13508,7 +13502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="12.9" customHeight="1">
+    <row r="9" spans="1:24" ht="12.95" customHeight="1">
       <c r="A9" s="198"/>
       <c r="B9" s="14">
         <v>1.2</v>
@@ -13577,7 +13571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="12.9" customHeight="1">
+    <row r="10" spans="1:24" ht="12.95" customHeight="1">
       <c r="A10" s="198"/>
       <c r="B10" s="14">
         <v>1.4</v>
@@ -13646,7 +13640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12.9" customHeight="1">
+    <row r="11" spans="1:24" ht="12.95" customHeight="1">
       <c r="A11" s="198"/>
       <c r="B11" s="14">
         <v>1.6</v>
@@ -13715,7 +13709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="12.9" customHeight="1">
+    <row r="12" spans="1:24" ht="12.95" customHeight="1">
       <c r="A12" s="198"/>
       <c r="B12" s="12">
         <v>1.8</v>
@@ -13784,7 +13778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="12.9" customHeight="1">
+    <row r="13" spans="1:24" ht="12.95" customHeight="1">
       <c r="A13" s="198"/>
       <c r="B13" s="12">
         <v>2</v>
@@ -13853,7 +13847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="12.9" customHeight="1">
+    <row r="14" spans="1:24" ht="12.95" customHeight="1">
       <c r="A14" s="198"/>
       <c r="B14" s="12">
         <v>3</v>
@@ -13922,7 +13916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12.9" customHeight="1">
+    <row r="15" spans="1:24" ht="12.95" customHeight="1">
       <c r="A15" s="198"/>
       <c r="B15" s="12">
         <v>4</v>
@@ -13991,7 +13985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12.9" customHeight="1">
+    <row r="16" spans="1:24" ht="12.95" customHeight="1">
       <c r="A16" s="198"/>
       <c r="B16" s="12">
         <v>5</v>
@@ -14060,7 +14054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="12.9" customHeight="1">
+    <row r="17" spans="1:23" ht="12.95" customHeight="1">
       <c r="A17" s="198"/>
       <c r="B17" s="12">
         <v>6</v>
@@ -14129,7 +14123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="12.9" customHeight="1">
+    <row r="18" spans="1:23" ht="12.95" customHeight="1">
       <c r="A18" s="198"/>
       <c r="B18" s="12">
         <v>7</v>
@@ -14198,7 +14192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="12.9" customHeight="1">
+    <row r="19" spans="1:23" ht="12.95" customHeight="1">
       <c r="A19" s="198"/>
       <c r="B19" s="12">
         <v>8</v>
@@ -14267,7 +14261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="12.9" customHeight="1">
+    <row r="20" spans="1:23" ht="12.95" customHeight="1">
       <c r="A20" s="198"/>
       <c r="B20" s="12">
         <v>9</v>
@@ -14336,7 +14330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="12.9" customHeight="1">
+    <row r="21" spans="1:23" ht="12.95" customHeight="1">
       <c r="A21" s="198"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -14405,7 +14399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="12.9" customHeight="1">
+    <row r="22" spans="1:23" ht="12.95" customHeight="1">
       <c r="A22" s="198"/>
       <c r="B22" s="12">
         <v>12</v>
@@ -14474,7 +14468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.9" customHeight="1">
+    <row r="23" spans="1:23" ht="12.95" customHeight="1">
       <c r="A23" s="198"/>
       <c r="B23" s="12">
         <v>14</v>
@@ -14543,7 +14537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="12.9" customHeight="1">
+    <row r="24" spans="1:23" ht="12.95" customHeight="1">
       <c r="A24" s="198"/>
       <c r="B24" s="12">
         <v>16</v>
@@ -14612,7 +14606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="12.9" customHeight="1">
+    <row r="25" spans="1:23" ht="12.95" customHeight="1">
       <c r="A25" s="198"/>
       <c r="B25" s="12">
         <v>18</v>
@@ -14681,7 +14675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="12.9" customHeight="1">
+    <row r="26" spans="1:23" ht="12.95" customHeight="1">
       <c r="A26" s="198"/>
       <c r="B26" s="12">
         <v>20</v>
@@ -14750,7 +14744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="12.9" customHeight="1">
+    <row r="27" spans="1:23" ht="12.95" customHeight="1">
       <c r="A27" s="198"/>
       <c r="B27" s="12">
         <v>22</v>
@@ -14819,7 +14813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="12.9" customHeight="1">
+    <row r="28" spans="1:23" ht="12.95" customHeight="1">
       <c r="A28" s="198"/>
       <c r="B28" s="12">
         <v>24</v>
@@ -14888,7 +14882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="12.9" customHeight="1">
+    <row r="29" spans="1:23" ht="12.95" customHeight="1">
       <c r="A29" s="198"/>
       <c r="B29" s="12">
         <v>26</v>
@@ -14957,7 +14951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="12.9" customHeight="1">
+    <row r="30" spans="1:23" ht="12.95" customHeight="1">
       <c r="A30" s="198"/>
       <c r="B30" s="12">
         <v>28</v>
@@ -15026,7 +15020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.9" customHeight="1">
+    <row r="31" spans="1:23" ht="12.95" customHeight="1">
       <c r="A31" s="198"/>
       <c r="B31" s="12">
         <v>100</v>
@@ -15121,13 +15115,13 @@
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="23" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -15160,7 +15154,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="41" t="s">
         <v>3</v>
@@ -15229,7 +15223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="12.9" customHeight="1">
+    <row r="3" spans="1:24" ht="12.95" customHeight="1">
       <c r="A3" s="198"/>
       <c r="B3" s="12">
         <v>0</v>
@@ -15298,7 +15292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="12.9" customHeight="1">
+    <row r="4" spans="1:24" ht="12.95" customHeight="1">
       <c r="A4" s="198"/>
       <c r="B4" s="24">
         <v>0.2</v>
@@ -15367,7 +15361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12.9" customHeight="1">
+    <row r="5" spans="1:24" ht="12.95" customHeight="1">
       <c r="A5" s="198"/>
       <c r="B5" s="26">
         <v>0.4</v>
@@ -15436,7 +15430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12.9" customHeight="1">
+    <row r="6" spans="1:24" ht="12.95" customHeight="1">
       <c r="A6" s="198"/>
       <c r="B6" s="26">
         <v>0.6</v>
@@ -15505,7 +15499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="12.9" customHeight="1">
+    <row r="7" spans="1:24" ht="12.95" customHeight="1">
       <c r="A7" s="198"/>
       <c r="B7" s="26">
         <v>0.8</v>
@@ -15574,7 +15568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="12.9" customHeight="1">
+    <row r="8" spans="1:24" ht="12.95" customHeight="1">
       <c r="A8" s="198"/>
       <c r="B8" s="14">
         <v>1</v>
@@ -15643,7 +15637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="12.9" customHeight="1">
+    <row r="9" spans="1:24" ht="12.95" customHeight="1">
       <c r="A9" s="198"/>
       <c r="B9" s="14">
         <v>1.2</v>
@@ -15712,7 +15706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="12.9" customHeight="1">
+    <row r="10" spans="1:24" ht="12.95" customHeight="1">
       <c r="A10" s="198"/>
       <c r="B10" s="14">
         <v>1.4</v>
@@ -15781,7 +15775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12.9" customHeight="1">
+    <row r="11" spans="1:24" ht="12.95" customHeight="1">
       <c r="A11" s="198"/>
       <c r="B11" s="14">
         <v>1.6</v>
@@ -15850,7 +15844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="12.9" customHeight="1">
+    <row r="12" spans="1:24" ht="12.95" customHeight="1">
       <c r="A12" s="198"/>
       <c r="B12" s="14">
         <v>1.8</v>
@@ -15919,7 +15913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="12.9" customHeight="1">
+    <row r="13" spans="1:24" ht="12.95" customHeight="1">
       <c r="A13" s="198"/>
       <c r="B13" s="12">
         <v>2</v>
@@ -15988,7 +15982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="12.9" customHeight="1">
+    <row r="14" spans="1:24" ht="12.95" customHeight="1">
       <c r="A14" s="198"/>
       <c r="B14" s="12">
         <v>3</v>
@@ -16057,7 +16051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12.9" customHeight="1">
+    <row r="15" spans="1:24" ht="12.95" customHeight="1">
       <c r="A15" s="198"/>
       <c r="B15" s="12">
         <v>4</v>
@@ -16126,7 +16120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12.9" customHeight="1">
+    <row r="16" spans="1:24" ht="12.95" customHeight="1">
       <c r="A16" s="198"/>
       <c r="B16" s="12">
         <v>5</v>
@@ -16195,7 +16189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="12.9" customHeight="1">
+    <row r="17" spans="1:23" ht="12.95" customHeight="1">
       <c r="A17" s="198"/>
       <c r="B17" s="12">
         <v>6</v>
@@ -16264,7 +16258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="12.9" customHeight="1">
+    <row r="18" spans="1:23" ht="12.95" customHeight="1">
       <c r="A18" s="198"/>
       <c r="B18" s="12">
         <v>7</v>
@@ -16333,7 +16327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="12.9" customHeight="1">
+    <row r="19" spans="1:23" ht="12.95" customHeight="1">
       <c r="A19" s="198"/>
       <c r="B19" s="12">
         <v>8</v>
@@ -16402,7 +16396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="12.9" customHeight="1">
+    <row r="20" spans="1:23" ht="12.95" customHeight="1">
       <c r="A20" s="198"/>
       <c r="B20" s="12">
         <v>9</v>
@@ -16471,7 +16465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="12.9" customHeight="1">
+    <row r="21" spans="1:23" ht="12.95" customHeight="1">
       <c r="A21" s="198"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -16540,7 +16534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="12.9" customHeight="1">
+    <row r="22" spans="1:23" ht="12.95" customHeight="1">
       <c r="A22" s="198"/>
       <c r="B22" s="12">
         <v>12</v>
@@ -16609,7 +16603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.9" customHeight="1">
+    <row r="23" spans="1:23" ht="12.95" customHeight="1">
       <c r="A23" s="198"/>
       <c r="B23" s="12">
         <v>14</v>
@@ -16678,7 +16672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="12.9" customHeight="1">
+    <row r="24" spans="1:23" ht="12.95" customHeight="1">
       <c r="A24" s="198"/>
       <c r="B24" s="12">
         <v>16</v>
@@ -16747,7 +16741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="12.9" customHeight="1">
+    <row r="25" spans="1:23" ht="12.95" customHeight="1">
       <c r="A25" s="198"/>
       <c r="B25" s="12">
         <v>18</v>
@@ -16816,7 +16810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="12.9" customHeight="1">
+    <row r="26" spans="1:23" ht="12.95" customHeight="1">
       <c r="A26" s="198"/>
       <c r="B26" s="12">
         <v>20</v>
@@ -16885,7 +16879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="12.9" customHeight="1">
+    <row r="27" spans="1:23" ht="12.95" customHeight="1">
       <c r="A27" s="198"/>
       <c r="B27" s="12">
         <v>22</v>
@@ -16954,7 +16948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="12.9" customHeight="1">
+    <row r="28" spans="1:23" ht="12.95" customHeight="1">
       <c r="A28" s="198"/>
       <c r="B28" s="12">
         <v>24</v>
@@ -17023,7 +17017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="12.9" customHeight="1">
+    <row r="29" spans="1:23" ht="12.95" customHeight="1">
       <c r="A29" s="198"/>
       <c r="B29" s="12">
         <v>26</v>
@@ -17092,7 +17086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="12.9" customHeight="1">
+    <row r="30" spans="1:23" ht="12.95" customHeight="1">
       <c r="A30" s="198"/>
       <c r="B30" s="12">
         <v>28</v>
@@ -17161,7 +17155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.9" customHeight="1">
+    <row r="31" spans="1:23" ht="12.95" customHeight="1">
       <c r="A31" s="198"/>
       <c r="B31" s="12">
         <v>100</v>
@@ -17257,16 +17251,16 @@
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="3" customWidth="1"/>
     <col min="9" max="22" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -17299,7 +17293,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="38" t="s">
         <v>21</v>
@@ -19396,16 +19390,16 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" style="3" customWidth="1"/>
-    <col min="9" max="22" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="3" customWidth="1"/>
+    <col min="9" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -19438,10 +19432,10 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C2" s="106">
         <v>0</v>
@@ -21529,16 +21523,16 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" style="3" customWidth="1"/>
-    <col min="9" max="22" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="3" customWidth="1"/>
+    <col min="9" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="16" customFormat="1" ht="18" customHeight="1">
@@ -21571,10 +21565,10 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:32" ht="13.2" thickBot="1">
+    <row r="2" spans="1:32" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -21847,7 +21841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="14.4">
+    <row r="6" spans="1:32" ht="15">
       <c r="A6" s="198"/>
       <c r="B6" s="26">
         <v>0.6</v>
@@ -21917,7 +21911,7 @@
       </c>
       <c r="AF6" s="163"/>
     </row>
-    <row r="7" spans="1:32" ht="15.6">
+    <row r="7" spans="1:32" ht="15.75">
       <c r="A7" s="198"/>
       <c r="B7" s="26">
         <v>0.8</v>
@@ -21987,7 +21981,7 @@
       </c>
       <c r="AF7" s="53"/>
     </row>
-    <row r="8" spans="1:32" ht="14.4">
+    <row r="8" spans="1:32" ht="15">
       <c r="A8" s="198"/>
       <c r="B8" s="34">
         <v>1</v>
@@ -22057,7 +22051,7 @@
       </c>
       <c r="AF8" s="163"/>
     </row>
-    <row r="9" spans="1:32" ht="14.4">
+    <row r="9" spans="1:32" ht="15">
       <c r="A9" s="198"/>
       <c r="B9" s="34">
         <v>1.2</v>
@@ -22127,7 +22121,7 @@
       </c>
       <c r="AF9" s="163"/>
     </row>
-    <row r="10" spans="1:32" ht="14.4">
+    <row r="10" spans="1:32" ht="15">
       <c r="A10" s="198"/>
       <c r="B10" s="34">
         <v>1.4</v>
@@ -22197,7 +22191,7 @@
       </c>
       <c r="AF10" s="163"/>
     </row>
-    <row r="11" spans="1:32" ht="14.4">
+    <row r="11" spans="1:32" ht="15">
       <c r="A11" s="198"/>
       <c r="B11" s="34">
         <v>1.6</v>
@@ -22267,7 +22261,7 @@
       </c>
       <c r="AF11" s="163"/>
     </row>
-    <row r="12" spans="1:32" ht="14.4">
+    <row r="12" spans="1:32" ht="15">
       <c r="A12" s="198"/>
       <c r="B12" s="34">
         <v>1.8</v>
@@ -22337,7 +22331,7 @@
       </c>
       <c r="AF12" s="163"/>
     </row>
-    <row r="13" spans="1:32" ht="15.6">
+    <row r="13" spans="1:32" ht="15.75">
       <c r="A13" s="198"/>
       <c r="B13" s="34">
         <v>2</v>
@@ -22407,7 +22401,7 @@
       </c>
       <c r="AF13" s="56"/>
     </row>
-    <row r="14" spans="1:32" ht="15.6">
+    <row r="14" spans="1:32" ht="15.75">
       <c r="A14" s="198"/>
       <c r="B14" s="34">
         <v>3</v>
@@ -22477,7 +22471,7 @@
       </c>
       <c r="AF14" s="56"/>
     </row>
-    <row r="15" spans="1:32" ht="14.4">
+    <row r="15" spans="1:32" ht="15">
       <c r="A15" s="198"/>
       <c r="B15" s="12">
         <v>4</v>
@@ -22547,7 +22541,7 @@
       </c>
       <c r="AF15" s="163"/>
     </row>
-    <row r="16" spans="1:32" ht="14.4">
+    <row r="16" spans="1:32" ht="15">
       <c r="A16" s="198"/>
       <c r="B16" s="12">
         <v>5</v>
@@ -22617,7 +22611,7 @@
       </c>
       <c r="AF16" s="163"/>
     </row>
-    <row r="17" spans="1:32" ht="14.4">
+    <row r="17" spans="1:32" ht="15">
       <c r="A17" s="198"/>
       <c r="B17" s="12">
         <v>6</v>
@@ -22687,7 +22681,7 @@
       </c>
       <c r="AF17" s="163"/>
     </row>
-    <row r="18" spans="1:32" ht="14.4">
+    <row r="18" spans="1:32" ht="15">
       <c r="A18" s="198"/>
       <c r="B18" s="12">
         <v>7</v>
@@ -22757,7 +22751,7 @@
       </c>
       <c r="AF18" s="163"/>
     </row>
-    <row r="19" spans="1:32" ht="14.4">
+    <row r="19" spans="1:32" ht="15">
       <c r="A19" s="198"/>
       <c r="B19" s="12">
         <v>8</v>
@@ -23668,27 +23662,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:U56"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" style="160" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="160" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="160" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="160" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="160" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="160" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="160" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="160" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" style="160" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="160" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.44140625" style="160" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.5546875" style="160" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="160" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="160" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.5703125" style="160" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="162" customFormat="1">
       <c r="A1" s="162" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B1" s="161" t="s">
         <v>24</v>
@@ -23703,16 +23697,16 @@
         <v>90</v>
       </c>
       <c r="F1" s="161" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="161" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="161" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="161" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="161" t="s">
-        <v>115</v>
-      </c>
       <c r="I1" s="161" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J1" s="161"/>
       <c r="K1" s="161"/>
@@ -23724,28 +23718,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="160" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="C2" s="160" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="D2" s="160" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="E2" s="160" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F2" s="160" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G2" s="160">
-        <v>255</v>
+        <v>200</v>
       </c>
       <c r="H2" s="160">
-        <v>229</v>
+        <v>128</v>
       </c>
       <c r="I2" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R2" s="160"/>
       <c r="S2" s="160"/>
@@ -23755,28 +23749,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="160" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="C3" s="160" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D3" s="160" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="E3" s="160" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F3" s="160" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="160">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H3" s="160">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="I3" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R3" s="160"/>
       <c r="S3" s="160"/>
@@ -23786,28 +23780,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="160" t="s">
-        <v>2</v>
+        <v>152</v>
       </c>
       <c r="C4" s="160" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="D4" s="160" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="E4" s="160" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="F4" s="160" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4" s="160">
-        <v>0</v>
+        <v>237</v>
       </c>
       <c r="H4" s="160">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="I4" s="160" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="R4" s="160"/>
       <c r="S4" s="160"/>
@@ -23817,28 +23811,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="160" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="C5" s="160" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="D5" s="160" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="E5" s="160" t="s">
-        <v>7</v>
+        <v>153</v>
       </c>
       <c r="F5" s="160" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="160">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="H5" s="160">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="I5" s="160" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="R5" s="160"/>
       <c r="S5" s="160"/>
@@ -23848,22 +23842,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="160" t="s">
-        <v>134</v>
+        <v>27</v>
       </c>
       <c r="C6" s="160" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="D6" s="160" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="160" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="160" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="160" t="s">
-        <v>125</v>
+      <c r="G6" s="160">
+        <v>174</v>
+      </c>
+      <c r="H6" s="160">
+        <v>212</v>
       </c>
       <c r="I6" s="160" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="R6" s="160"/>
       <c r="S6" s="160"/>
@@ -23873,22 +23873,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="160" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="C7" s="160" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="D7" s="160" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="160" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="160" t="s">
-        <v>156</v>
-      </c>
-      <c r="F7" s="160" t="s">
-        <v>125</v>
+      <c r="G7" s="160">
+        <v>255</v>
+      </c>
+      <c r="H7" s="160">
+        <v>153</v>
       </c>
       <c r="I7" s="160" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="R7" s="160"/>
       <c r="S7" s="160"/>
@@ -23898,22 +23904,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="160" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="C8" s="160" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="D8" s="160" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="E8" s="160" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="F8" s="160" t="s">
-        <v>125</v>
+        <v>123</v>
+      </c>
+      <c r="G8" s="160">
+        <v>2</v>
+      </c>
+      <c r="H8" s="160">
+        <v>127</v>
       </c>
       <c r="I8" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R8" s="160"/>
       <c r="S8" s="160"/>
@@ -23923,28 +23935,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="160" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="C9" s="160" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="D9" s="160" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="E9" s="160" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F9" s="160" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G9" s="160">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="H9" s="160">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="I9" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R9" s="160"/>
       <c r="S9" s="160"/>
@@ -23954,28 +23966,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="160" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C10" s="160" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D10" s="160" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="E10" s="160" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F10" s="160" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G10" s="160">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="H10" s="160">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="I10" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R10" s="160"/>
       <c r="S10" s="160"/>
@@ -23985,28 +23997,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="160" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="C11" s="160" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="D11" s="160" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="E11" s="160" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F11" s="160" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G11" s="160">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H11" s="160">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="I11" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R11" s="160"/>
       <c r="S11" s="160"/>
@@ -24016,28 +24028,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="160" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C12" s="160" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D12" s="160" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="E12" s="160" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F12" s="160" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G12" s="160">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="H12" s="160">
-        <v>154</v>
+        <v>229</v>
       </c>
       <c r="I12" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R12" s="160"/>
       <c r="S12" s="160"/>
@@ -24047,28 +24059,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="160" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C13" s="160" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D13" s="160" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="E13" s="160" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F13" s="160" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G13" s="160">
-        <v>223</v>
+        <v>120</v>
       </c>
       <c r="H13" s="160">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="I13" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R13" s="160"/>
       <c r="S13" s="160"/>
@@ -24078,22 +24090,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="160" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C14" s="160" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="160" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="E14" s="160" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="F14" s="160" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="G14" s="160">
+        <v>0</v>
+      </c>
+      <c r="H14" s="160">
+        <v>0</v>
       </c>
       <c r="I14" s="160" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="R14" s="160"/>
       <c r="S14" s="160"/>
@@ -24103,22 +24121,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="160" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C15" s="160" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="D15" s="160" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="E15" s="160" t="s">
-        <v>151</v>
+        <v>7</v>
       </c>
       <c r="F15" s="160" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="G15" s="160">
+        <v>0</v>
+      </c>
+      <c r="H15" s="160">
+        <v>0</v>
       </c>
       <c r="I15" s="160" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="R15" s="160"/>
       <c r="S15" s="160"/>
@@ -24128,28 +24152,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="160" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C16" s="160" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D16" s="160" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="E16" s="160" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="F16" s="160" t="s">
-        <v>127</v>
-      </c>
-      <c r="G16" s="160">
-        <v>211</v>
-      </c>
-      <c r="H16" s="160">
-        <v>199</v>
+        <v>123</v>
       </c>
       <c r="I16" s="160" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="R16" s="160"/>
       <c r="S16" s="160"/>
@@ -24159,28 +24177,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="160" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="C17" s="160" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="D17" s="160" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="E17" s="160" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="F17" s="160" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" s="160">
-        <v>128</v>
-      </c>
-      <c r="H17" s="160">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I17" s="160" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="R17" s="160"/>
       <c r="S17" s="160"/>
@@ -24190,28 +24202,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="160" t="s">
-        <v>14</v>
+        <v>135</v>
       </c>
       <c r="C18" s="160" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="D18" s="160" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="E18" s="160" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="F18" s="160" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="160">
-        <v>177</v>
-      </c>
-      <c r="H18" s="160">
-        <v>211</v>
+        <v>123</v>
       </c>
       <c r="I18" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R18" s="160"/>
       <c r="S18" s="160"/>
@@ -24221,28 +24227,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="160" t="s">
-        <v>16</v>
+        <v>145</v>
       </c>
       <c r="C19" s="160" t="s">
-        <v>57</v>
+        <v>146</v>
       </c>
       <c r="D19" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="160" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F19" s="160" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G19" s="160">
-        <v>255</v>
+        <v>26</v>
       </c>
       <c r="H19" s="160">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="I19" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R19" s="160"/>
       <c r="S19" s="160"/>
@@ -24252,28 +24258,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="160" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C20" s="160" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="D20" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="160" t="s">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F20" s="160" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G20" s="160">
-        <v>255</v>
+        <v>191</v>
       </c>
       <c r="H20" s="160">
-        <v>179</v>
+        <v>111</v>
       </c>
       <c r="I20" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R20" s="160"/>
       <c r="S20" s="160"/>
@@ -24283,28 +24289,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="160" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C21" s="160" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D21" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="160" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F21" s="160" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="160">
         <v>127</v>
       </c>
-      <c r="G21" s="160">
-        <v>178</v>
-      </c>
       <c r="H21" s="160">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="I21" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R21" s="160"/>
       <c r="S21" s="160"/>
@@ -24314,22 +24320,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="160" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C22" s="160" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E22" s="160" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="160" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="G22" s="160">
+        <v>61</v>
+      </c>
+      <c r="H22" s="160">
+        <v>154</v>
       </c>
       <c r="I22" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R22" s="160"/>
       <c r="S22" s="160"/>
@@ -24339,22 +24351,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="160" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="C23" s="160" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="D23" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E23" s="160" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="F23" s="160" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="G23" s="160">
+        <v>223</v>
+      </c>
+      <c r="H23" s="160">
+        <v>138</v>
       </c>
       <c r="I23" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R23" s="160"/>
       <c r="S23" s="160"/>
@@ -24364,28 +24382,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="160" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="C24" s="160" t="s">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="D24" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E24" s="160" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="F24" s="160" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" s="160">
-        <v>222</v>
-      </c>
-      <c r="H24" s="160">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="I24" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R24" s="160"/>
       <c r="S24" s="160"/>
@@ -24395,22 +24407,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="160" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="C25" s="160" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D25" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E25" s="160" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="F25" s="160" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I25" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R25" s="160"/>
       <c r="S25" s="160"/>
@@ -24420,28 +24432,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="160" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="C26" s="160" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="D26" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E26" s="160" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="F26" s="160" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G26" s="160">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="H26" s="160">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="I26" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R26" s="160"/>
       <c r="S26" s="160"/>
@@ -24451,28 +24463,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="160" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" s="160" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D27" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E27" s="160" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="F27" s="160" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G27" s="160">
-        <v>217</v>
+        <v>255</v>
       </c>
       <c r="H27" s="160">
-        <v>217</v>
+        <v>153</v>
       </c>
       <c r="I27" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R27" s="160"/>
       <c r="S27" s="160"/>
@@ -24482,28 +24494,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="160" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C28" s="160" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="D28" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E28" s="160" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="F28" s="160" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G28" s="160">
-        <v>180</v>
+        <v>255</v>
       </c>
       <c r="H28" s="160">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="I28" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R28" s="160"/>
       <c r="S28" s="160"/>
@@ -24513,28 +24525,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="160" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="C29" s="160" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="D29" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E29" s="160" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F29" s="160" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G29" s="160">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="H29" s="160">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="I29" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R29" s="160"/>
       <c r="S29" s="160"/>
@@ -24544,28 +24556,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="160" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C30" s="160" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D30" s="160" t="s">
         <v>91</v>
       </c>
       <c r="E30" s="160" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="F30" s="160" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G30" s="160">
-        <v>237</v>
+        <v>128</v>
       </c>
       <c r="H30" s="160">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I30" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R30" s="160"/>
       <c r="S30" s="160"/>
@@ -24575,28 +24587,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="160" t="s">
-        <v>154</v>
+        <v>10</v>
       </c>
       <c r="C31" s="160" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="D31" s="160" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="E31" s="160" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="F31" s="160" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G31" s="160">
-        <v>237</v>
+        <v>178</v>
       </c>
       <c r="H31" s="160">
-        <v>111</v>
+        <v>214</v>
       </c>
       <c r="I31" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R31" s="160"/>
       <c r="S31" s="160"/>
@@ -24606,28 +24618,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="160" t="s">
-        <v>155</v>
+        <v>9</v>
       </c>
       <c r="C32" s="160" t="s">
-        <v>158</v>
+        <v>50</v>
       </c>
       <c r="D32" s="160" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="E32" s="160" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="F32" s="160" t="s">
-        <v>126</v>
-      </c>
-      <c r="G32" s="160">
-        <v>235</v>
-      </c>
-      <c r="H32" s="160">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="I32" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R32" s="160"/>
       <c r="S32" s="160"/>
@@ -24637,28 +24643,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="160" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="C33" s="160" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="D33" s="160" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="E33" s="160" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="F33" s="160" t="s">
         <v>126</v>
       </c>
-      <c r="G33" s="160">
-        <v>0</v>
-      </c>
-      <c r="H33" s="160">
-        <v>200</v>
-      </c>
       <c r="I33" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R33" s="160"/>
       <c r="S33" s="160"/>
@@ -24668,28 +24668,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="160" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="C34" s="160" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="D34" s="160" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="E34" s="160" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="F34" s="160" t="s">
         <v>126</v>
       </c>
       <c r="G34" s="160">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="H34" s="160">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="I34" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R34" s="160"/>
       <c r="S34" s="160"/>
@@ -24699,28 +24699,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="160" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="C35" s="160" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="D35" s="160" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E35" s="160" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="F35" s="160" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G35" s="160">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="H35" s="160">
-        <v>134</v>
+        <v>229</v>
       </c>
       <c r="I35" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R35" s="160"/>
       <c r="S35" s="160"/>
@@ -24730,28 +24730,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="160" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C36" s="160" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="D36" s="160" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="E36" s="160" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="F36" s="160" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="160">
-        <v>174</v>
-      </c>
-      <c r="H36" s="160">
-        <v>212</v>
+        <v>126</v>
       </c>
       <c r="I36" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R36" s="160"/>
       <c r="S36" s="160"/>
@@ -24761,28 +24755,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="160" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C37" s="160" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D37" s="160" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="E37" s="160" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F37" s="160" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G37" s="160">
-        <v>255</v>
+        <v>128</v>
       </c>
       <c r="H37" s="160">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="I37" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R37" s="160"/>
       <c r="S37" s="160"/>
@@ -24792,28 +24786,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="160" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C38" s="160" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="D38" s="160" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="E38" s="160" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="F38" s="160" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G38" s="160">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="H38" s="160">
-        <v>127</v>
+        <v>217</v>
       </c>
       <c r="I38" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R38" s="160"/>
       <c r="S38" s="160"/>
@@ -24823,28 +24817,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="160" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C39" s="160" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="D39" s="160" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="E39" s="160" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="F39" s="160" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G39" s="160">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="H39" s="160">
-        <v>176</v>
+        <v>98</v>
       </c>
       <c r="I39" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R39" s="160"/>
       <c r="S39" s="160"/>
@@ -24854,28 +24848,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="160" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="C40" s="160" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D40" s="160" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="E40" s="160" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="F40" s="160" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G40" s="160">
-        <v>201</v>
+        <v>237</v>
       </c>
       <c r="H40" s="160">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="I40" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R40" s="160"/>
       <c r="S40" s="160"/>
@@ -24885,28 +24879,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="160" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C41" s="160" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="D41" s="160" t="s">
-        <v>160</v>
-      </c>
-      <c r="E41" s="160" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="F41" s="160" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G41" s="160">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="H41" s="160">
-        <v>102</v>
+        <v>179</v>
       </c>
       <c r="I41" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R41" s="160"/>
       <c r="S41" s="160"/>
@@ -24922,19 +24913,19 @@
         <v>110</v>
       </c>
       <c r="D42" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F42" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G42" s="160">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="H42" s="160">
-        <v>179</v>
+        <v>2</v>
       </c>
       <c r="I42" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R42" s="160"/>
       <c r="S42" s="160"/>
@@ -24944,25 +24935,25 @@
         <v>42</v>
       </c>
       <c r="B43" s="160" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="C43" s="160" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="D43" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F43" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G43" s="160">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="H43" s="160">
         <v>2</v>
       </c>
       <c r="I43" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R43" s="160"/>
       <c r="S43" s="160"/>
@@ -24972,25 +24963,25 @@
         <v>43</v>
       </c>
       <c r="B44" s="160" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C44" s="160" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D44" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F44" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G44" s="160">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="H44" s="160">
-        <v>2</v>
+        <v>138</v>
       </c>
       <c r="I44" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R44" s="160"/>
       <c r="S44" s="160"/>
@@ -25000,25 +24991,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="160" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C45" s="160" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="D45" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F45" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G45" s="160">
-        <v>41</v>
+        <v>166</v>
       </c>
       <c r="H45" s="160">
-        <v>138</v>
+        <v>30</v>
       </c>
       <c r="I45" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R45" s="160"/>
       <c r="S45" s="160"/>
@@ -25028,25 +25019,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="160" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C46" s="160" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="D46" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F46" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G46" s="160">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H46" s="160">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="I46" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R46" s="160"/>
       <c r="S46" s="160"/>
@@ -25056,25 +25047,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="160" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C47" s="160" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D47" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F47" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G47" s="160">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="H47" s="160">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="I47" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R47" s="160"/>
       <c r="S47" s="160"/>
@@ -25084,25 +25075,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="160" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C48" s="160" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D48" s="160" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F48" s="160" t="s">
-        <v>126</v>
-      </c>
-      <c r="G48" s="160">
-        <v>118</v>
-      </c>
-      <c r="H48" s="160">
-        <v>29</v>
-      </c>
-      <c r="I48" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R48" s="160"/>
       <c r="S48" s="160"/>
@@ -25112,16 +25094,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="160" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="C49" s="160" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="D49" s="160" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F49" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R49" s="160"/>
       <c r="S49" s="160"/>
@@ -25131,16 +25113,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="160" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C50" s="160" t="s">
         <v>161</v>
       </c>
       <c r="D50" s="160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F50" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R50" s="160"/>
       <c r="S50" s="160"/>
@@ -25156,10 +25138,10 @@
         <v>163</v>
       </c>
       <c r="D51" s="160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F51" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R51" s="160"/>
       <c r="S51" s="160"/>
@@ -25175,10 +25157,10 @@
         <v>165</v>
       </c>
       <c r="D52" s="160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F52" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R52" s="160"/>
       <c r="S52" s="160"/>
@@ -25194,10 +25176,10 @@
         <v>167</v>
       </c>
       <c r="D53" s="160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F53" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R53" s="160"/>
       <c r="S53" s="160"/>
@@ -25213,10 +25195,10 @@
         <v>169</v>
       </c>
       <c r="D54" s="160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F54" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R54" s="160"/>
       <c r="S54" s="160"/>
@@ -25232,36 +25214,17 @@
         <v>171</v>
       </c>
       <c r="D55" s="160" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F55" s="160" t="s">
-        <v>126</v>
-      </c>
-      <c r="R55" s="160"/>
-      <c r="S55" s="160"/>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" s="160" t="s">
-        <v>172</v>
-      </c>
-      <c r="C56" s="160" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" s="160" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" s="160" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K47">
-    <sortCondition ref="D2:D47"/>
-    <sortCondition ref="J2:J47"/>
-    <sortCondition ref="B2:B47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:K46">
+    <sortCondition ref="D12:D46"/>
+    <sortCondition ref="J12:J46"/>
+    <sortCondition ref="B12:B46"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -25284,17 +25247,17 @@
       <selection activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="22" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -25327,7 +25290,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="43" t="s">
         <v>12</v>
@@ -27424,11 +27387,11 @@
       <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -27461,7 +27424,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="16.2" thickBot="1">
+    <row r="2" spans="1:24" ht="16.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="45" t="s">
         <v>14</v>
@@ -29557,15 +29520,15 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="1" max="1" width="3.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -29598,7 +29561,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="46" t="s">
         <v>16</v>
@@ -31694,18 +31657,18 @@
       <selection activeCell="AC50" sqref="AC50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="22" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="3" max="3" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="22" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -31738,7 +31701,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="42" t="s">
         <v>11</v>
@@ -33834,12 +33797,12 @@
       <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -33872,7 +33835,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="44" t="s">
         <v>10</v>
@@ -35968,13 +35931,13 @@
       <selection activeCell="AD42" sqref="AD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="22" width="5.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -36007,7 +35970,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="40" t="s">
         <v>9</v>
@@ -38121,16 +38084,16 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="16" customFormat="1" ht="18" customHeight="1">
@@ -38163,10 +38126,10 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:31" ht="13.2" thickBot="1">
+    <row r="2" spans="1:31" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -38232,7 +38195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.4">
+    <row r="3" spans="1:31" ht="15">
       <c r="A3" s="198"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -38302,7 +38265,7 @@
       </c>
       <c r="AE3" s="163"/>
     </row>
-    <row r="4" spans="1:31" ht="15.6">
+    <row r="4" spans="1:31" ht="15.75">
       <c r="A4" s="198"/>
       <c r="B4" s="8">
         <v>0.2</v>
@@ -38372,7 +38335,7 @@
       </c>
       <c r="AE4" s="53"/>
     </row>
-    <row r="5" spans="1:31" ht="14.4">
+    <row r="5" spans="1:31" ht="15">
       <c r="A5" s="198"/>
       <c r="B5" s="34">
         <v>0.4</v>
@@ -38442,7 +38405,7 @@
       </c>
       <c r="AE5" s="163"/>
     </row>
-    <row r="6" spans="1:31" ht="14.4">
+    <row r="6" spans="1:31" ht="15">
       <c r="A6" s="198"/>
       <c r="B6" s="34">
         <v>0.6</v>
@@ -38512,7 +38475,7 @@
       </c>
       <c r="AE6" s="163"/>
     </row>
-    <row r="7" spans="1:31" ht="14.4">
+    <row r="7" spans="1:31" ht="15">
       <c r="A7" s="198"/>
       <c r="B7" s="34">
         <v>0.8</v>
@@ -38582,7 +38545,7 @@
       </c>
       <c r="AE7" s="163"/>
     </row>
-    <row r="8" spans="1:31" ht="14.4">
+    <row r="8" spans="1:31" ht="15">
       <c r="A8" s="198"/>
       <c r="B8" s="34">
         <v>1</v>
@@ -38652,7 +38615,7 @@
       </c>
       <c r="AE8" s="163"/>
     </row>
-    <row r="9" spans="1:31" ht="14.4">
+    <row r="9" spans="1:31" ht="15">
       <c r="A9" s="198"/>
       <c r="B9" s="34">
         <v>1.2</v>
@@ -38722,7 +38685,7 @@
       </c>
       <c r="AE9" s="163"/>
     </row>
-    <row r="10" spans="1:31" ht="15.6">
+    <row r="10" spans="1:31" ht="15.75">
       <c r="A10" s="198"/>
       <c r="B10" s="34">
         <v>1.4</v>
@@ -38792,7 +38755,7 @@
       </c>
       <c r="AE10" s="56"/>
     </row>
-    <row r="11" spans="1:31" ht="15.6">
+    <row r="11" spans="1:31" ht="15.75">
       <c r="A11" s="198"/>
       <c r="B11" s="26">
         <v>1.6</v>
@@ -38862,7 +38825,7 @@
       </c>
       <c r="AE11" s="56"/>
     </row>
-    <row r="12" spans="1:31" ht="14.4">
+    <row r="12" spans="1:31" ht="15">
       <c r="A12" s="198"/>
       <c r="B12" s="26">
         <v>1.8</v>
@@ -38932,7 +38895,7 @@
       </c>
       <c r="AE12" s="163"/>
     </row>
-    <row r="13" spans="1:31" ht="14.4">
+    <row r="13" spans="1:31" ht="15">
       <c r="A13" s="198"/>
       <c r="B13" s="26">
         <v>2</v>
@@ -39002,7 +38965,7 @@
       </c>
       <c r="AE13" s="163"/>
     </row>
-    <row r="14" spans="1:31" ht="14.4">
+    <row r="14" spans="1:31" ht="15">
       <c r="A14" s="198"/>
       <c r="B14" s="26">
         <v>3</v>
@@ -39072,7 +39035,7 @@
       </c>
       <c r="AE14" s="163"/>
     </row>
-    <row r="15" spans="1:31" ht="14.4">
+    <row r="15" spans="1:31" ht="15">
       <c r="A15" s="198"/>
       <c r="B15" s="24">
         <v>4</v>
@@ -39142,7 +39105,7 @@
       </c>
       <c r="AE15" s="163"/>
     </row>
-    <row r="16" spans="1:31" ht="14.4">
+    <row r="16" spans="1:31" ht="15">
       <c r="A16" s="198"/>
       <c r="B16" s="26">
         <v>5</v>
@@ -40267,16 +40230,16 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1">
@@ -40309,10 +40272,10 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:28" ht="15" thickBot="1">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -40379,7 +40342,7 @@
       </c>
       <c r="AB2" s="163"/>
     </row>
-    <row r="3" spans="1:28" ht="15.6">
+    <row r="3" spans="1:28" ht="15.75">
       <c r="A3" s="198"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -40449,7 +40412,7 @@
       </c>
       <c r="AB3" s="53"/>
     </row>
-    <row r="4" spans="1:28" ht="14.4">
+    <row r="4" spans="1:28" ht="15">
       <c r="A4" s="198"/>
       <c r="B4" s="8">
         <v>0.2</v>
@@ -40519,7 +40482,7 @@
       </c>
       <c r="AB4" s="163"/>
     </row>
-    <row r="5" spans="1:28" ht="14.4">
+    <row r="5" spans="1:28" ht="15">
       <c r="A5" s="198"/>
       <c r="B5" s="8">
         <v>0.4</v>
@@ -40589,7 +40552,7 @@
       </c>
       <c r="AB5" s="163"/>
     </row>
-    <row r="6" spans="1:28" ht="14.4">
+    <row r="6" spans="1:28" ht="15">
       <c r="A6" s="198"/>
       <c r="B6" s="8">
         <v>0.6</v>
@@ -40659,7 +40622,7 @@
       </c>
       <c r="AB6" s="163"/>
     </row>
-    <row r="7" spans="1:28" ht="14.4">
+    <row r="7" spans="1:28" ht="15">
       <c r="A7" s="198"/>
       <c r="B7" s="8">
         <v>0.8</v>
@@ -40729,7 +40692,7 @@
       </c>
       <c r="AB7" s="163"/>
     </row>
-    <row r="8" spans="1:28" ht="14.4">
+    <row r="8" spans="1:28" ht="15">
       <c r="A8" s="198"/>
       <c r="B8" s="8">
         <v>1</v>
@@ -40799,7 +40762,7 @@
       </c>
       <c r="AB8" s="163"/>
     </row>
-    <row r="9" spans="1:28" ht="15.6">
+    <row r="9" spans="1:28" ht="15.75">
       <c r="A9" s="198"/>
       <c r="B9" s="8">
         <v>1.2</v>
@@ -40869,7 +40832,7 @@
       </c>
       <c r="AB9" s="56"/>
     </row>
-    <row r="10" spans="1:28" ht="15.6">
+    <row r="10" spans="1:28" ht="15.75">
       <c r="A10" s="198"/>
       <c r="B10" s="8">
         <v>1.4</v>
@@ -40939,7 +40902,7 @@
       </c>
       <c r="AB10" s="56"/>
     </row>
-    <row r="11" spans="1:28" ht="14.4">
+    <row r="11" spans="1:28" ht="15">
       <c r="A11" s="198"/>
       <c r="B11" s="34">
         <v>1.6</v>
@@ -41009,7 +40972,7 @@
       </c>
       <c r="AB11" s="163"/>
     </row>
-    <row r="12" spans="1:28" ht="14.4">
+    <row r="12" spans="1:28" ht="15">
       <c r="A12" s="198"/>
       <c r="B12" s="34">
         <v>1.8</v>
@@ -41079,7 +41042,7 @@
       </c>
       <c r="AB12" s="163"/>
     </row>
-    <row r="13" spans="1:28" ht="14.4">
+    <row r="13" spans="1:28" ht="15">
       <c r="A13" s="198"/>
       <c r="B13" s="34">
         <v>2</v>
@@ -41149,7 +41112,7 @@
       </c>
       <c r="AB13" s="163"/>
     </row>
-    <row r="14" spans="1:28" ht="14.4">
+    <row r="14" spans="1:28" ht="15">
       <c r="A14" s="198"/>
       <c r="B14" s="26">
         <v>3</v>
@@ -41219,7 +41182,7 @@
       </c>
       <c r="AB14" s="163"/>
     </row>
-    <row r="15" spans="1:28" ht="14.4">
+    <row r="15" spans="1:28" ht="15">
       <c r="A15" s="198"/>
       <c r="B15" s="26">
         <v>4</v>
@@ -42413,15 +42376,15 @@
       <selection activeCell="B2" sqref="B2:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.6640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.7109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -42454,7 +42417,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
         <v>15</v>
@@ -44549,16 +44512,16 @@
       <selection sqref="A1:W31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
-    <col min="9" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="9" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1">
@@ -44591,10 +44554,10 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:28" ht="15" thickBot="1">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -44661,7 +44624,7 @@
       </c>
       <c r="AB2" s="163"/>
     </row>
-    <row r="3" spans="1:28" ht="15.6">
+    <row r="3" spans="1:28" ht="15.75">
       <c r="A3" s="198"/>
       <c r="B3" s="8">
         <v>0</v>
@@ -44731,7 +44694,7 @@
       </c>
       <c r="AB3" s="53"/>
     </row>
-    <row r="4" spans="1:28" ht="14.4">
+    <row r="4" spans="1:28" ht="15">
       <c r="A4" s="198"/>
       <c r="B4" s="8">
         <v>0.2</v>
@@ -44801,7 +44764,7 @@
       </c>
       <c r="AB4" s="163"/>
     </row>
-    <row r="5" spans="1:28" ht="14.4">
+    <row r="5" spans="1:28" ht="15">
       <c r="A5" s="198"/>
       <c r="B5" s="8">
         <v>0.4</v>
@@ -44871,7 +44834,7 @@
       </c>
       <c r="AB5" s="163"/>
     </row>
-    <row r="6" spans="1:28" ht="14.4">
+    <row r="6" spans="1:28" ht="15">
       <c r="A6" s="198"/>
       <c r="B6" s="8">
         <v>0.6</v>
@@ -44941,7 +44904,7 @@
       </c>
       <c r="AB6" s="163"/>
     </row>
-    <row r="7" spans="1:28" ht="14.4">
+    <row r="7" spans="1:28" ht="15">
       <c r="A7" s="198"/>
       <c r="B7" s="34">
         <v>0.8</v>
@@ -45011,7 +44974,7 @@
       </c>
       <c r="AB7" s="163"/>
     </row>
-    <row r="8" spans="1:28" ht="14.4">
+    <row r="8" spans="1:28" ht="15">
       <c r="A8" s="198"/>
       <c r="B8" s="34">
         <v>1</v>
@@ -45081,7 +45044,7 @@
       </c>
       <c r="AB8" s="163"/>
     </row>
-    <row r="9" spans="1:28" ht="15.6">
+    <row r="9" spans="1:28" ht="15.75">
       <c r="A9" s="198"/>
       <c r="B9" s="34">
         <v>1.2</v>
@@ -45151,7 +45114,7 @@
       </c>
       <c r="AB9" s="56"/>
     </row>
-    <row r="10" spans="1:28" ht="15.6">
+    <row r="10" spans="1:28" ht="15.75">
       <c r="A10" s="198"/>
       <c r="B10" s="34">
         <v>1.4</v>
@@ -45221,7 +45184,7 @@
       </c>
       <c r="AB10" s="56"/>
     </row>
-    <row r="11" spans="1:28" ht="14.4">
+    <row r="11" spans="1:28" ht="15">
       <c r="A11" s="198"/>
       <c r="B11" s="34">
         <v>1.6</v>
@@ -45291,7 +45254,7 @@
       </c>
       <c r="AB11" s="163"/>
     </row>
-    <row r="12" spans="1:28" ht="14.4">
+    <row r="12" spans="1:28" ht="15">
       <c r="A12" s="198"/>
       <c r="B12" s="34">
         <v>1.8</v>
@@ -45361,7 +45324,7 @@
       </c>
       <c r="AB12" s="163"/>
     </row>
-    <row r="13" spans="1:28" ht="14.4">
+    <row r="13" spans="1:28" ht="15">
       <c r="A13" s="198"/>
       <c r="B13" s="26">
         <v>2</v>
@@ -45431,7 +45394,7 @@
       </c>
       <c r="AB13" s="163"/>
     </row>
-    <row r="14" spans="1:28" ht="14.4">
+    <row r="14" spans="1:28" ht="15">
       <c r="A14" s="198"/>
       <c r="B14" s="26">
         <v>3</v>
@@ -45501,7 +45464,7 @@
       </c>
       <c r="AB14" s="163"/>
     </row>
-    <row r="15" spans="1:28" ht="14.4">
+    <row r="15" spans="1:28" ht="15">
       <c r="A15" s="198"/>
       <c r="B15" s="24">
         <v>4</v>
@@ -46694,41 +46657,41 @@
       <selection pane="topRight" activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" style="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="52" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" style="64" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="64" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="52" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="52" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.85546875" style="52" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8" style="52" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="30" max="34" width="10.6640625" style="52" customWidth="1"/>
-    <col min="35" max="16384" width="10.88671875" style="52"/>
+    <col min="26" max="26" width="9.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="8.140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="30" max="34" width="10.7109375" style="52" customWidth="1"/>
+    <col min="35" max="16384" width="10.85546875" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="31.2">
+    <row r="1" spans="1:35" ht="31.5">
       <c r="A1" s="51" t="s">
         <v>22</v>
       </c>
@@ -46817,25 +46780,25 @@
         <v>19</v>
       </c>
       <c r="AD1" s="163" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AE1" s="163" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF1" s="163" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG1" s="163" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH1" s="163" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI1" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="AF1" s="163" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG1" s="163" t="s">
-        <v>141</v>
-      </c>
-      <c r="AH1" s="163" t="s">
-        <v>143</v>
-      </c>
-      <c r="AI1" s="52" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" s="53" customFormat="1" ht="31.2">
+    </row>
+    <row r="2" spans="1:35" s="53" customFormat="1" ht="31.5">
       <c r="A2" s="49" t="s">
         <v>23</v>
       </c>
@@ -48309,15 +48272,15 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -48350,7 +48313,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="78" t="s">
         <v>18</v>
@@ -50445,14 +50408,14 @@
       <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="3" max="17" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -50485,7 +50448,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="47" t="s">
         <v>17</v>
@@ -52580,17 +52543,17 @@
       <selection activeCell="AA52" sqref="AA52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="1" customWidth="1"/>
     <col min="4" max="7" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="17" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="23" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -52623,7 +52586,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="48" t="s">
         <v>20</v>
@@ -54279,7 +54242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="13.2" thickBot="1">
+    <row r="26" spans="1:23" ht="13.5" thickBot="1">
       <c r="A26" s="198"/>
       <c r="B26" s="11">
         <v>20</v>
@@ -54348,7 +54311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="13.2" thickTop="1">
+    <row r="27" spans="1:23" ht="13.5" thickTop="1">
       <c r="A27" s="198"/>
       <c r="B27" s="143">
         <v>22</v>
@@ -54624,7 +54587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="13.2" thickBot="1">
+    <row r="31" spans="1:23" ht="13.5" thickBot="1">
       <c r="A31" s="198"/>
       <c r="B31" s="145">
         <v>30</v>
@@ -54693,7 +54656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="13.2" thickTop="1">
+    <row r="32" spans="1:23" ht="13.5" thickTop="1">
       <c r="B32" s="1">
         <v>35</v>
       </c>
@@ -54992,13 +54955,13 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="116" bestFit="1" customWidth="1"/>
-    <col min="3" max="22" width="4.88671875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.109375" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="1"/>
+    <col min="1" max="1" width="4.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="116" bestFit="1" customWidth="1"/>
+    <col min="3" max="22" width="4.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="5.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -55031,7 +54994,7 @@
       <c r="W1" s="204"/>
       <c r="X1" s="17"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="205"/>
       <c r="B2" s="113" t="s">
         <v>19</v>
@@ -56066,7 +56029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="13.2" thickBot="1">
+    <row r="17" spans="1:23" ht="13.5" thickBot="1">
       <c r="A17" s="205"/>
       <c r="B17" s="115">
         <v>6</v>
@@ -56135,7 +56098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="13.2" thickTop="1">
+    <row r="18" spans="1:23" ht="13.5" thickTop="1">
       <c r="A18" s="205"/>
       <c r="B18" s="152">
         <v>7</v>
@@ -56894,7 +56857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="13.2" thickBot="1">
+    <row r="29" spans="1:23" ht="13.5" thickBot="1">
       <c r="A29" s="205"/>
       <c r="B29" s="156">
         <v>26</v>
@@ -56963,7 +56926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="13.2" thickTop="1">
+    <row r="30" spans="1:23" ht="13.5" thickTop="1">
       <c r="A30" s="205"/>
       <c r="B30" s="114">
         <v>28</v>
@@ -57125,7 +57088,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="198" t="s">
@@ -57156,7 +57119,7 @@
       <c r="V1" s="199"/>
       <c r="W1" s="199"/>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="48" t="s">
         <v>87</v>
@@ -59524,7 +59487,7 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
   </cols>
@@ -59558,7 +59521,7 @@
       <c r="V1" s="199"/>
       <c r="W1" s="199"/>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="48" t="s">
         <v>86</v>
@@ -61927,7 +61890,7 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="206" t="s">
@@ -61958,7 +61921,7 @@
       <c r="V1" s="207"/>
       <c r="W1" s="207"/>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="A2" s="206"/>
       <c r="B2" s="128" t="s">
         <v>88</v>
@@ -64323,13 +64286,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -64406,13 +64369,13 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D4">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -64452,19 +64415,19 @@
         <v>0.30499999999999999</v>
       </c>
       <c r="B6">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="C6">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D6">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="E6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -64498,19 +64461,19 @@
         <v>0.61</v>
       </c>
       <c r="B8">
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="C8">
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="D8">
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="E8">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="F8">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -64521,13 +64484,13 @@
         <v>0.76249999999999996</v>
       </c>
       <c r="B9">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="C9">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="D9">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="E9">
         <v>0.6</v>
@@ -64576,10 +64539,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.4</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F11">
-        <v>0.4</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="G11">
         <v>0.6</v>
@@ -64590,19 +64553,19 @@
         <v>1.22</v>
       </c>
       <c r="B12">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="C12">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="D12">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="E12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0.4</v>
@@ -64613,22 +64576,22 @@
         <v>1.3725000000000001</v>
       </c>
       <c r="B13">
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="C13">
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="D13">
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="E13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0.2</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -64787,9 +64750,9 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" s="126" customFormat="1" ht="43.2">
+    <row r="1" spans="1:9" s="126" customFormat="1" ht="60">
       <c r="A1" s="125" t="s">
         <v>80</v>
       </c>
@@ -64800,10 +64763,10 @@
         <v>84</v>
       </c>
       <c r="D1" s="123" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E1" s="124" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F1" s="124" t="s">
         <v>81</v>
@@ -64815,7 +64778,7 @@
         <v>83</v>
       </c>
       <c r="I1" s="124" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="126" customFormat="1">
@@ -66096,11 +66059,11 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="22" width="5.6640625" customWidth="1"/>
-    <col min="23" max="23" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="22" width="5.7109375" customWidth="1"/>
+    <col min="23" max="23" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -68359,11 +68322,11 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" style="99" customWidth="1"/>
-    <col min="3" max="23" width="6.88671875" style="104" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="99" customWidth="1"/>
+    <col min="3" max="23" width="6.85546875" style="104" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -68391,7 +68354,7 @@
       <c r="V1" s="197"/>
       <c r="W1" s="197"/>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="B2" s="105" t="s">
         <v>35</v>
       </c>
@@ -70623,14 +70586,14 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="95" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="95" customWidth="1"/>
     <col min="4" max="4" width="11" style="95" customWidth="1"/>
-    <col min="5" max="22" width="8.109375" style="95" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" style="95" customWidth="1"/>
+    <col min="5" max="22" width="8.140625" style="95" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" style="95" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -72892,10 +72855,10 @@
       <selection sqref="A1:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
@@ -72904,7 +72867,7 @@
     <col min="18" max="18" width="4" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="22" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="5.44140625" style="3"/>
+    <col min="24" max="16384" width="5.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="16" customFormat="1" ht="18" customHeight="1">
@@ -72937,7 +72900,7 @@
       <c r="W1" s="199"/>
       <c r="X1" s="65"/>
     </row>
-    <row r="2" spans="1:24" ht="13.2" thickBot="1">
+    <row r="2" spans="1:24" ht="13.5" thickBot="1">
       <c r="A2" s="198"/>
       <c r="B2" s="71" t="s">
         <v>7</v>
@@ -75029,7 +74992,7 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="200" t="s">
@@ -75060,7 +75023,7 @@
       <c r="V1" s="201"/>
       <c r="W1" s="201"/>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="A2" s="200"/>
       <c r="B2" s="190" t="s">
         <v>87</v>
@@ -77423,7 +77386,7 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="200" t="s">
@@ -77454,7 +77417,7 @@
       <c r="V1" s="201"/>
       <c r="W1" s="201"/>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1">
       <c r="A2" s="200"/>
       <c r="B2" s="190" t="s">
         <v>87</v>

</xml_diff>